<commit_message>
Non Augmented test data experiments conducted, checkpoints saved
</commit_message>
<xml_diff>
--- a/Baseline ViT Comparison.xlsx
+++ b/Baseline ViT Comparison.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/39d0109d20b3edff/Desktop/ECE699/Code/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/39d0109d20b3edff/Desktop/ECE699/Debiased ViT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="165" documentId="11_F25DC773A252ABDACC104810E99C7D565ADE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{395EA198-5A85-487A-8932-70FDA44F28DF}"/>
+  <xr:revisionPtr revIDLastSave="210" documentId="11_F25DC773A252ABDACC104810E99C7D565ADE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{52B484DA-6393-4074-BBC5-BD07C7890F25}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13866" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1727" yWindow="1727" windowWidth="19200" windowHeight="10033" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Hyper Parameters</t>
   </si>
@@ -72,22 +72,31 @@
     <t>Basic ViT</t>
   </si>
   <si>
-    <t xml:space="preserve">learning_rate = 0.001  weight_decay = 0.0001  optimizer_type = Adam  scheduler = fixed  patience = 5  grad_norm_clip = 1  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">learning_rate = 0.001  weight_decay = 0.0001  scheduler = CosineAnnealingLR  patience = 5  grad_norm_clip = 1  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">learning_rate = 0.001  weight_decay = 0.0001  optimizer_type = SGD  scheduler = fixed  patience = 5  grad_norm_clip = 1  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">batch_size = 32  optimizer = SGD  learning_rate = 0.001  scheduler = fixed patience = 5  grad_norm_clip = 1  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">batch_size = 32  optimizer = SGD  learning_rate = 0.001  scheduler = CosineAnnealingLR patience = 5  grad_norm_clip = 1  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">batch_size = 32  optimizer = Adam  learning_rate = 0.001  scheduler = fixed patience = 5  grad_norm_clip = 1  </t>
+    <t xml:space="preserve">learning_rate = 0.001  optimizer = SGD  scheduler = fixed  max_stop_count = 5  grad_norm_clip = 1  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">learning_rate = 0.001  optimizer = SGD  scheduler = CosineAnnealingLR  max_stop_count = 5  grad_norm_clip = 1  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">learning_rate = 0.001  optimizer = Adam  scheduler = fixed  max_stop_count = 5  grad_norm_clip = 1  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">optimizer = Adam  learning_rate = 0.001  scheduler = fixed   max_stop_count = 5  grad_norm_clip = 1  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">optimizer = SGD  learning_rate = 0.001  scheduler = CosineAnnealingLR   max_stop_count = 5  grad_norm_clip = 1  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">optimizer = SGD  learning_rate = 0.001  scheduler = fixed   max_stop_count = 5  grad_norm_clip = 1  </t>
+  </si>
+  <si>
+    <t>CNN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">batch_size = 512  optimizer = Adam  learning_rate = 0.001  scheduler = fixed  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">batch_size = 512  optimizer = SGD  learning_rate = 0.001  scheduler = CosineAnnealingLR  </t>
   </si>
 </sst>
 </file>
@@ -131,10 +140,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -419,15 +427,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:M15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="57.76171875" customWidth="1"/>
+    <col min="1" max="1" width="95.9375" customWidth="1"/>
     <col min="3" max="3" width="12.64453125" customWidth="1"/>
     <col min="4" max="4" width="11.76171875" customWidth="1"/>
   </cols>
@@ -480,43 +488,43 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B4">
-        <v>0.58699999999999997</v>
+        <v>0.6109</v>
       </c>
       <c r="C4">
-        <v>0.57289999999999996</v>
+        <v>0.65620000000000001</v>
       </c>
       <c r="D4">
-        <v>0.60070000000000001</v>
+        <v>0.56710000000000005</v>
       </c>
       <c r="E4">
-        <v>0.58099999999999996</v>
+        <v>0.59430000000000005</v>
       </c>
       <c r="F4">
-        <v>0.57689999999999997</v>
+        <v>0.62380000000000002</v>
       </c>
       <c r="G4">
-        <v>0.58679999999999999</v>
+        <v>0.61170000000000002</v>
       </c>
       <c r="H4">
-        <v>0.5645</v>
+        <v>0.6129</v>
       </c>
       <c r="I4">
-        <v>0.57579999999999998</v>
+        <v>0.60609999999999997</v>
       </c>
       <c r="J4">
-        <v>0.55169999999999997</v>
+        <v>0.62070000000000003</v>
       </c>
       <c r="K4">
-        <v>0.59379999999999999</v>
+        <v>0.6452</v>
       </c>
       <c r="L4">
-        <v>0.58460000000000001</v>
+        <v>0.625</v>
       </c>
       <c r="M4">
-        <v>0.56369999999999998</v>
+        <v>0.61339999999999995</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.5">
@@ -524,81 +532,81 @@
         <v>16</v>
       </c>
       <c r="B5" s="1">
-        <v>0.81230000000000002</v>
+        <v>0.80720000000000003</v>
       </c>
       <c r="C5">
-        <v>0.77080000000000004</v>
+        <v>0.78469999999999995</v>
       </c>
       <c r="D5">
-        <v>0.85229999999999995</v>
+        <v>0.82889999999999997</v>
       </c>
       <c r="E5">
-        <v>0.83460000000000001</v>
+        <v>0.81589999999999996</v>
       </c>
       <c r="F5">
-        <v>0.8014</v>
+        <v>0.8</v>
       </c>
       <c r="G5">
-        <v>0.81159999999999999</v>
+        <v>0.80679999999999996</v>
       </c>
       <c r="H5" s="1">
-        <v>0.8226</v>
+        <v>0.80649999999999999</v>
       </c>
       <c r="I5">
-        <v>0.78790000000000004</v>
+        <v>0.72729999999999995</v>
       </c>
       <c r="J5">
-        <v>0.86209999999999998</v>
+        <v>0.89659999999999995</v>
       </c>
       <c r="K5">
-        <v>0.86670000000000003</v>
+        <v>0.88890000000000002</v>
       </c>
       <c r="L5">
-        <v>0.82540000000000002</v>
+        <v>0.8</v>
       </c>
       <c r="M5">
-        <v>0.82499999999999996</v>
+        <v>0.81189999999999996</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B6">
-        <v>0.79859999999999998</v>
+        <v>0.81230000000000002</v>
       </c>
       <c r="C6">
         <v>0.82289999999999996</v>
       </c>
       <c r="D6">
-        <v>0.7752</v>
+        <v>0.80200000000000005</v>
       </c>
       <c r="E6">
-        <v>0.77959999999999996</v>
+        <v>0.80069999999999997</v>
       </c>
       <c r="F6">
-        <v>0.80069999999999997</v>
+        <v>0.81159999999999999</v>
       </c>
       <c r="G6">
-        <v>0.79900000000000004</v>
+        <v>0.8125</v>
       </c>
       <c r="H6">
-        <v>0.7581</v>
+        <v>0.7258</v>
       </c>
       <c r="I6">
-        <v>0.84850000000000003</v>
+        <v>0.78790000000000004</v>
       </c>
       <c r="J6">
         <v>0.6552</v>
       </c>
       <c r="K6">
-        <v>0.73680000000000001</v>
+        <v>0.72219999999999995</v>
       </c>
       <c r="L6">
-        <v>0.78869999999999996</v>
+        <v>0.75360000000000005</v>
       </c>
       <c r="M6">
-        <v>0.75180000000000002</v>
+        <v>0.72150000000000003</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.5">
@@ -611,40 +619,40 @@
         <v>18</v>
       </c>
       <c r="B9">
-        <v>0.78500000000000003</v>
+        <v>0.53069999999999995</v>
       </c>
       <c r="C9">
-        <v>0.77429999999999999</v>
+        <v>0.95140000000000002</v>
       </c>
       <c r="D9">
-        <v>0.79530000000000001</v>
+        <v>0.1242</v>
       </c>
       <c r="E9">
-        <v>0.78520000000000001</v>
+        <v>0.5121</v>
       </c>
       <c r="F9">
-        <v>0.77969999999999995</v>
+        <v>0.66590000000000005</v>
       </c>
       <c r="G9">
-        <v>0.78480000000000005</v>
+        <v>0.53779999999999994</v>
       </c>
       <c r="H9">
-        <v>0.7258</v>
+        <v>0.5484</v>
       </c>
       <c r="I9">
-        <v>0.69699999999999995</v>
+        <v>0.96970000000000001</v>
       </c>
       <c r="J9">
-        <v>0.75860000000000005</v>
+        <v>6.9000000000000006E-2</v>
       </c>
       <c r="K9">
-        <v>0.76670000000000005</v>
+        <v>0.54239999999999999</v>
       </c>
       <c r="L9">
-        <v>0.73019999999999996</v>
+        <v>0.69569999999999999</v>
       </c>
       <c r="M9">
-        <v>0.7278</v>
+        <v>0.51929999999999998</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.5">
@@ -657,7 +665,7 @@
       <c r="C10">
         <v>0.75349999999999995</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10">
         <v>0.81879999999999997</v>
       </c>
       <c r="E10">
@@ -693,40 +701,127 @@
         <v>20</v>
       </c>
       <c r="B11">
-        <v>0.53069999999999995</v>
+        <v>0.78500000000000003</v>
       </c>
       <c r="C11">
-        <v>0.95140000000000002</v>
+        <v>0.77429999999999999</v>
       </c>
       <c r="D11">
-        <v>0.1242</v>
+        <v>0.79530000000000001</v>
       </c>
       <c r="E11">
-        <v>0.5121</v>
+        <v>0.78520000000000001</v>
       </c>
       <c r="F11">
-        <v>0.66590000000000005</v>
+        <v>0.77969999999999995</v>
       </c>
       <c r="G11">
-        <v>0.53779999999999994</v>
+        <v>0.78480000000000005</v>
       </c>
       <c r="H11">
-        <v>0.5484</v>
+        <v>0.7258</v>
       </c>
       <c r="I11">
-        <v>0.96970000000000001</v>
+        <v>0.69699999999999995</v>
       </c>
       <c r="J11">
-        <v>6.9000000000000006E-2</v>
+        <v>0.75860000000000005</v>
       </c>
       <c r="K11">
-        <v>0.54239999999999999</v>
+        <v>0.76670000000000005</v>
       </c>
       <c r="L11">
-        <v>0.69569999999999999</v>
+        <v>0.73019999999999996</v>
       </c>
       <c r="M11">
-        <v>0.51929999999999998</v>
+        <v>0.7278</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.5">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.5">
+      <c r="A14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14">
+        <v>0.68769999999999998</v>
+      </c>
+      <c r="C14">
+        <v>0.875</v>
+      </c>
+      <c r="D14">
+        <v>0.50670000000000004</v>
+      </c>
+      <c r="E14">
+        <v>0.63160000000000005</v>
+      </c>
+      <c r="F14">
+        <v>0.73360000000000003</v>
+      </c>
+      <c r="G14">
+        <v>0.69089999999999996</v>
+      </c>
+      <c r="H14">
+        <v>0.7258</v>
+      </c>
+      <c r="I14">
+        <v>0.93940000000000001</v>
+      </c>
+      <c r="J14">
+        <v>0.48280000000000001</v>
+      </c>
+      <c r="K14">
+        <v>0.67390000000000005</v>
+      </c>
+      <c r="L14">
+        <v>0.78480000000000005</v>
+      </c>
+      <c r="M14">
+        <v>0.71109999999999995</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.5">
+      <c r="A15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15">
+        <v>0.7833</v>
+      </c>
+      <c r="C15">
+        <v>0.76390000000000002</v>
+      </c>
+      <c r="D15">
+        <v>0.80200000000000005</v>
+      </c>
+      <c r="E15">
+        <v>0.78849999999999998</v>
+      </c>
+      <c r="F15">
+        <v>0.77600000000000002</v>
+      </c>
+      <c r="G15">
+        <v>0.78300000000000003</v>
+      </c>
+      <c r="H15">
+        <v>0.7419</v>
+      </c>
+      <c r="I15">
+        <v>0.72729999999999995</v>
+      </c>
+      <c r="J15">
+        <v>0.75860000000000005</v>
+      </c>
+      <c r="K15">
+        <v>0.7742</v>
+      </c>
+      <c r="L15">
+        <v>0.75</v>
+      </c>
+      <c r="M15">
+        <v>0.7429</v>
       </c>
     </row>
   </sheetData>

</xml_diff>